<commit_message>
Agregado calculos y Vista para modelo MaterialForro
</commit_message>
<xml_diff>
--- a/Documentos/Detalles Desarrollo.xlsx
+++ b/Documentos/Detalles Desarrollo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resultado Finales" sheetId="1" r:id="rId1"/>
@@ -759,9 +759,6 @@
     <t>Costo en tela extra</t>
   </si>
   <si>
-    <t>Multiplicacion (Costo metro tela * Cantidad metro tela)</t>
-  </si>
-  <si>
     <t>RIB utilizado</t>
   </si>
   <si>
@@ -799,6 +796,9 @@
   </si>
   <si>
     <t>Calculo del tiempo de trabajo en jornada normal (M. Obra) TABLA: TiempoTrabajo</t>
+  </si>
+  <si>
+    <t>Multiplicacion (Costo metro tela * Cantidad de Tela extra)</t>
   </si>
 </sst>
 </file>
@@ -1947,10 +1947,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="96" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="96" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="30" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="52" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
@@ -2459,20 +2459,27 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C65" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>100</v>
+      </c>
+      <c r="H67">
+        <f>+F67*12</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>230</v>
       </c>
@@ -2482,8 +2489,11 @@
       <c r="D68" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>59</v>
       </c>
@@ -2494,7 +2504,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>208</v>
       </c>
@@ -2505,7 +2515,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>210</v>
       </c>
@@ -2516,7 +2526,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>236</v>
       </c>
@@ -2527,9 +2537,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C73" t="s">
         <v>14</v>
@@ -2538,7 +2548,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>239</v>
       </c>
@@ -2549,7 +2559,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>240</v>
       </c>
@@ -2560,7 +2570,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>242</v>
       </c>
@@ -2568,51 +2578,51 @@
         <v>14</v>
       </c>
       <c r="D76" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
-        <v>244</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B79" s="28" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B79" s="28" t="s">
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" t="s">
         <v>246</v>
       </c>
-      <c r="C79" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C80" t="s">
         <v>14</v>
       </c>
       <c r="D80" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2629,8 +2639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2643,7 +2653,7 @@
   <sheetData>
     <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
@@ -2999,7 +3009,7 @@
     </row>
     <row r="45" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A45" s="38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B45" s="38"/>
       <c r="C45" s="38"/>

</xml_diff>

<commit_message>
Agregado modulos de calculos
</commit_message>
<xml_diff>
--- a/Documentos/Detalles Desarrollo.xlsx
+++ b/Documentos/Detalles Desarrollo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Resultado Finales" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="276">
   <si>
     <t>TIPO ING.</t>
   </si>
@@ -417,15 +417,6 @@
     <t>Total Sueldo</t>
   </si>
   <si>
-    <t>Suma (Total Sueldo Fijo + Total Sueldo Variable)</t>
-  </si>
-  <si>
-    <t>Suma (Horas Extras + Premios)</t>
-  </si>
-  <si>
-    <t>Suma (Sueldo Fijo + IESS)</t>
-  </si>
-  <si>
     <t>Tasa</t>
   </si>
   <si>
@@ -435,9 +426,6 @@
     <t>Extradia de Modelo Calculo del tiempo de trabajo en jornada normal (M. Obra)</t>
   </si>
   <si>
-    <t>Division (Total Sueldo / Minutos Trabajados por persona al anio)</t>
-  </si>
-  <si>
     <t>Total Tasa</t>
   </si>
   <si>
@@ -558,9 +546,6 @@
     <t>Tasa de Gastos de Fabricacion</t>
   </si>
   <si>
-    <t>Suma (Gastos de aministacion + Gastos por operaciones + Mantenimientos + Otros Gastos + Egresos no operativos + Ventas 12 Meses)</t>
-  </si>
-  <si>
     <t>Costo de Gastos de Administracion</t>
   </si>
   <si>
@@ -615,9 +600,6 @@
     <t>Multiplicacion (Costo * Tasa de Gastos de Ventas)</t>
   </si>
   <si>
-    <t>Gastos de Ventas (M. Obra) - TABLA: Gasto Venta</t>
-  </si>
-  <si>
     <t>Gastos de Administracion (M. Obra) - TABLA: GastoAdmin</t>
   </si>
   <si>
@@ -789,16 +771,91 @@
     <t>Tiempo de produccion en minutos por prenda  (M. OBRA) - TABLA: TiempoProdPrenda</t>
   </si>
   <si>
-    <t>Costo Materia Prima Extra (REND. M.P.E) - Tabla: MateriaExtra</t>
-  </si>
-  <si>
-    <t>Costo Materia Prima Forro (M.P.D. FORROS) Tabla: MateriaForros</t>
-  </si>
-  <si>
     <t>Calculo del tiempo de trabajo en jornada normal (M. Obra) TABLA: TiempoTrabajo</t>
   </si>
   <si>
     <t>Multiplicacion (Costo metro tela * Cantidad de Tela extra)</t>
+  </si>
+  <si>
+    <t>Rendimientos y Costo Materia Prima Extra (REND. M.P.E.) - Tabla : MateriaPrimaExtra</t>
+  </si>
+  <si>
+    <t>Costo Materia Prima Forro (M.P.D. FORROS) - Tabla: MateriaForros</t>
+  </si>
+  <si>
+    <t>Nombre Materia Prima</t>
+  </si>
+  <si>
+    <t>Char</t>
+  </si>
+  <si>
+    <t>Relacional (Tabla Talla)</t>
+  </si>
+  <si>
+    <t>Relacional (Tabla Tela)</t>
+  </si>
+  <si>
+    <t>Largo Extra</t>
+  </si>
+  <si>
+    <t>Ancho Extra</t>
+  </si>
+  <si>
+    <t>Extraida de la tabla Tela</t>
+  </si>
+  <si>
+    <t>Costo Tela</t>
+  </si>
+  <si>
+    <t>Piezas Reales</t>
+  </si>
+  <si>
+    <t>Redondeo inmediato inferior (0,5 de presición)</t>
+  </si>
+  <si>
+    <t>Cantidad tela a utilizar</t>
+  </si>
+  <si>
+    <t>Division (Ancho Tela / Ancho Extra)</t>
+  </si>
+  <si>
+    <t>Suma (Largo Extra + Scrap)</t>
+  </si>
+  <si>
+    <t>Division ((Largo Extra * Costo Tela) / Piezas Reales)</t>
+  </si>
+  <si>
+    <t>Multiplicacion (Redondear inmediato superior entero (1 / Piezas Reales) * Largo total</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Costo Materia Prima Extra (REND. M.P.E) - Tabla: MateriaPrimaExtra</t>
+  </si>
+  <si>
+    <t>Gastos de Ventas (M. Obra) - TABLA: GastoVenta</t>
+  </si>
+  <si>
+    <t>Suma (Gastos de aministacion + Gastos por operaciones + Mantenimientos + Otros Gastos + Egresos no operativos)</t>
+  </si>
+  <si>
+    <t>hr.employee</t>
+  </si>
+  <si>
+    <t>Minutos Producidos al año</t>
+  </si>
+  <si>
+    <t>Suma (Sueldo Fijo + IESS) hr.employe</t>
+  </si>
+  <si>
+    <t>Suma (Horas Extras + Premios) hr.employe</t>
+  </si>
+  <si>
+    <t>Suma (Total Sueldo Fijo + Total Sueldo Variable) hr.employe</t>
+  </si>
+  <si>
+    <t>Division (Total Sueldo / Minutos Trabajados por persona al anio) hr.employe</t>
   </si>
 </sst>
 </file>
@@ -874,7 +931,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -959,6 +1016,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -972,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1006,6 +1069,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1019,6 +1083,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1338,12 +1405,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="A1" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1537,13 +1604,13 @@
         <v>29</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1551,7 +1618,7 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -1565,7 +1632,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>13</v>
@@ -1576,7 +1643,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>13</v>
@@ -1652,7 +1719,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1663,12 +1730,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="A1" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -1795,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -1947,10 +2014,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="96" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView zoomScale="96" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1961,12 +2028,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -2183,12 +2250,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A30" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
+      <c r="A30" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
@@ -2203,10 +2270,10 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C33" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -2233,7 +2300,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
@@ -2241,7 +2308,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C37" t="s">
         <v>50</v>
@@ -2249,7 +2316,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C38" t="s">
         <v>50</v>
@@ -2262,13 +2329,13 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
         <v>207</v>
-      </c>
-      <c r="C42" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -2279,82 +2346,82 @@
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B49" s="27" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A52" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
+      <c r="A52" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
@@ -2369,7 +2436,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -2391,7 +2458,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C57" t="s">
         <v>50</v>
@@ -2399,7 +2466,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C58" t="s">
         <v>50</v>
@@ -2407,7 +2474,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C59" t="s">
         <v>50</v>
@@ -2418,7 +2485,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C60" t="s">
         <v>50</v>
@@ -2429,7 +2496,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C61" t="s">
         <v>50</v>
@@ -2437,7 +2504,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C62" t="s">
         <v>50</v>
@@ -2453,7 +2520,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C64" t="s">
         <v>50</v>
@@ -2461,7 +2528,7 @@
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C65" t="s">
         <v>50</v>
@@ -2481,13 +2548,13 @@
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C68" t="s">
         <v>50</v>
       </c>
       <c r="D68" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F68">
         <v>12</v>
@@ -2501,135 +2568,308 @@
         <v>50</v>
       </c>
       <c r="D69" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C71" t="s">
         <v>14</v>
       </c>
       <c r="D71" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C72" t="s">
         <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C73" t="s">
         <v>14</v>
       </c>
       <c r="D73" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C74" t="s">
         <v>13</v>
       </c>
       <c r="D74" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C75" t="s">
         <v>14</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C76" t="s">
         <v>14</v>
       </c>
       <c r="D76" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B79" s="28" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C79" t="s">
         <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C80" t="s">
         <v>14</v>
       </c>
       <c r="D80" t="s">
-        <v>250</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="A83" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="B83" s="35"/>
+      <c r="C83" s="35"/>
+      <c r="D83" s="35"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>38</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>202</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>258</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>256</v>
+      </c>
+      <c r="C91" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>255</v>
+      </c>
+      <c r="C92" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B95" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>224</v>
+      </c>
+      <c r="C96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>204</v>
+      </c>
+      <c r="C97" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C98" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" t="s">
+        <v>260</v>
+      </c>
+      <c r="G98">
+        <v>10</v>
+      </c>
+      <c r="H98">
+        <v>100</v>
+      </c>
+      <c r="J98">
+        <f>+G98*H99</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>261</v>
+      </c>
+      <c r="C99" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" t="s">
+        <v>265</v>
+      </c>
+      <c r="G99" t="s">
+        <v>266</v>
+      </c>
+      <c r="H99">
+        <v>12</v>
+      </c>
+      <c r="J99">
+        <f>+J98/H98</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B100" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C100" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A83:D83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2639,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D99"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2652,12 +2892,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
-        <v>252</v>
-      </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="A2" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -2703,14 +2943,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="8" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2752,68 +2992,68 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="16" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="24" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2821,12 +3061,12 @@
       <c r="D20" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
+      <c r="A22" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
@@ -2846,6 +3086,9 @@
       <c r="C24" t="s">
         <v>65</v>
       </c>
+      <c r="D24" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -2854,6 +3097,9 @@
       <c r="C25" t="s">
         <v>65</v>
       </c>
+      <c r="D25" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
@@ -2862,6 +3108,9 @@
       <c r="C26" t="s">
         <v>50</v>
       </c>
+      <c r="D26" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
@@ -2870,6 +3119,9 @@
       <c r="C27" t="s">
         <v>50</v>
       </c>
+      <c r="D27" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
@@ -2878,6 +3130,9 @@
       <c r="C28" t="s">
         <v>50</v>
       </c>
+      <c r="D28" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
@@ -2886,10 +3141,13 @@
       <c r="C29" t="s">
         <v>50</v>
       </c>
+      <c r="D29" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
         <v>50</v>
@@ -2897,10 +3155,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2916,7 +3177,7 @@
         <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>131</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2927,7 +3188,7 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>130</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -2938,62 +3199,62 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -3004,16 +3265,16 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A45" s="38" t="s">
-        <v>255</v>
-      </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
+      <c r="A45" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
@@ -3028,7 +3289,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
         <v>50</v>
@@ -3036,7 +3297,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
         <v>50</v>
@@ -3044,9 +3305,17 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>271</v>
+      </c>
+      <c r="C50" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3057,33 +3326,33 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B54" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A57" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="B57" s="39"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
+      <c r="A57" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="41"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
@@ -3098,42 +3367,42 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -3143,33 +3412,33 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C66" t="s">
         <v>14</v>
       </c>
       <c r="D66" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B67" s="17" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C67" t="s">
         <v>14</v>
       </c>
       <c r="D67" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A70" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
+      <c r="A70" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
@@ -3184,58 +3453,58 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C72" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C74" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C77" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C78" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -3245,33 +3514,33 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C82" t="s">
         <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>176</v>
+        <v>269</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B83" s="19" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C83" t="s">
         <v>14</v>
       </c>
       <c r="D83" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A86" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="B86" s="35"/>
-      <c r="C86" s="35"/>
-      <c r="D86" s="35"/>
+      <c r="A86" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
@@ -3286,58 +3555,58 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C88" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C89" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C90" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C91" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C92" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C93" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C94" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.2">
@@ -3347,24 +3616,24 @@
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C98" t="s">
         <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B99" s="23" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C99" t="s">
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>